<commit_message>
Fix trade options player cycling issue, update trade priority rule set
</commit_message>
<xml_diff>
--- a/src/NRL_stats.xlsx
+++ b/src/NRL_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rossritchie/code/fantasy_trade_calculator/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F6A5DE-36C5-294D-A3B5-263600E062A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F80393D3-AAF7-D742-A888-88BFA94A4391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41560" yWindow="3600" windowWidth="22880" windowHeight="17260" xr2:uid="{B4242749-2F31-BC4D-9D1D-C0882BBF0A2E}"/>
+    <workbookView xWindow="33460" yWindow="2540" windowWidth="29980" windowHeight="18340" xr2:uid="{B4242749-2F31-BC4D-9D1D-C0882BBF0A2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="2" r:id="rId1"/>
@@ -2063,16 +2063,16 @@
   <dimension ref="A1:AL815"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E819" sqref="E819"/>
+      <selection pane="bottomRight" activeCell="H816" sqref="H816"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="6" width="10.83203125" customWidth="1"/>
-    <col min="13" max="34" width="0" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="13" max="34" width="10.83203125" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="35" max="35" width="10.83203125" collapsed="1"/>
     <col min="36" max="38" width="10.83203125" style="2"/>
   </cols>
@@ -3880,7 +3880,7 @@
         <v>-26.883211678832119</v>
       </c>
     </row>
-    <row r="33" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -15876,7 +15876,7 @@
         <v>-17.941605839416056</v>
       </c>
     </row>
-    <row r="259" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A259">
         <f t="shared" ref="A259:A272" si="12">A258</f>
         <v>1</v>
@@ -24013,7 +24013,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="411" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A411">
         <v>2</v>
       </c>
@@ -29059,7 +29059,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="504" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="504" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
       <c r="A504">
         <v>2</v>
       </c>
@@ -38845,7 +38845,7 @@
         <v>5.1642335766423386</v>
       </c>
     </row>
-    <row r="687" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
+    <row r="687" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A687">
         <v>3</v>
       </c>
@@ -43596,7 +43596,7 @@
         <v>-6.7591240875912426</v>
       </c>
     </row>
-    <row r="775" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="775" spans="1:38" hidden="1" x14ac:dyDescent="0.2">
       <c r="A775">
         <v>3</v>
       </c>
@@ -45728,7 +45728,7 @@
   <autoFilter ref="A1:AL815" xr:uid="{7B1841C9-D21C-2040-9467-2F510B1F6134}">
     <filterColumn colId="1">
       <filters>
-        <filter val="Jaxson Paulo"/>
+        <filter val="C. Townsend"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
add (tentative) DPP functionality
</commit_message>
<xml_diff>
--- a/src/NRL_stats.xlsx
+++ b/src/NRL_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rossritchie/code/fantasy_trade_calculator/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C31D77-3F60-9740-9A36-DD659D48DB59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD43FA14-85FD-CB4C-BA74-E7E1F5996F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32300" yWindow="3520" windowWidth="31400" windowHeight="17420" xr2:uid="{B4242749-2F31-BC4D-9D1D-C0882BBF0A2E}"/>
+    <workbookView xWindow="35080" yWindow="2580" windowWidth="31400" windowHeight="17420" xr2:uid="{B4242749-2F31-BC4D-9D1D-C0882BBF0A2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="2" r:id="rId1"/>
@@ -1217,7 +1217,7 @@
     <t/>
   </si>
   <si>
-    <t>POS</t>
+    <t>POS1</t>
   </si>
 </sst>
 </file>
@@ -2115,10 +2115,10 @@
   <dimension ref="A1:AO832"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomRight" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
abort optimising - calculate trades function not finding traded out players in database
</commit_message>
<xml_diff>
--- a/src/NRL_stats.xlsx
+++ b/src/NRL_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rossritchie/code/fantasy_trade_calculator/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F38055-7C16-0A40-9233-0C40B508DA01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC4E10EB-7950-5F4F-B555-C38ACBCB1ECC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33680" yWindow="2340" windowWidth="31400" windowHeight="17420" xr2:uid="{B4242749-2F31-BC4D-9D1D-C0882BBF0A2E}"/>
+    <workbookView xWindow="35400" yWindow="2340" windowWidth="31400" windowHeight="17420" xr2:uid="{B4242749-2F31-BC4D-9D1D-C0882BBF0A2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="2" r:id="rId1"/>
@@ -1214,10 +1214,10 @@
     <t>POS1</t>
   </si>
   <si>
-    <t>Tota_ base</t>
+    <t>Base exceeds price premium</t>
   </si>
   <si>
-    <t>Base_exceeds_price_premium</t>
+    <t>Total base</t>
   </si>
 </sst>
 </file>
@@ -1725,7 +1725,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -1736,6 +1736,12 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -2118,56 +2124,58 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AQ11" sqref="AQ11"/>
+      <selection pane="bottomRight" activeCell="AP7" sqref="AP7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="9" width="10.83203125" customWidth="1"/>
-    <col min="11" max="11" width="20" customWidth="1"/>
+    <col min="10" max="11" width="10.6640625" customWidth="1"/>
+    <col min="12" max="15" width="0" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="16" max="37" width="10.83203125" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="38" max="38" width="10.83203125" collapsed="1"/>
-    <col min="39" max="41" width="10.83203125" style="2"/>
+    <col min="38" max="38" width="0" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="39" max="39" width="10.83203125" style="2" collapsed="1"/>
+    <col min="40" max="41" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:41" s="10" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
         <v>345</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="10" t="s">
         <v>371</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="10" t="s">
         <v>369</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="10" t="s">
         <v>391</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="10" t="s">
         <v>389</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="I1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="I1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="L1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="L1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="10" t="s">
         <v>7</v>
       </c>
       <c r="P1" s="3" t="s">
@@ -2236,11 +2244,12 @@
       <c r="AK1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AM1" s="11" t="s">
+        <v>393</v>
+      </c>
+      <c r="AN1" s="11"/>
+      <c r="AO1" s="11" t="s">
         <v>392</v>
-      </c>
-      <c r="AO1" s="2" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.2">

</xml_diff>